<commit_message>
added table showing the pattern lining up over A mod 60 for #5 V1
</commit_message>
<xml_diff>
--- a/consolidated_data.xlsx
+++ b/consolidated_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Q5 Comparison A2" sheetId="17" r:id="rId5"/>
     <sheet name="Q6" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Comparing differences A mod 60" sheetId="18" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>DP</t>
   </si>
@@ -66,13 +67,27 @@
   <si>
     <t>DFF DP-Greedy c2</t>
   </si>
+  <si>
+    <t>Difference of Greedy vs DP for V1 where max is 60</t>
+  </si>
+  <si>
+    <t>A % 60</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -114,30 +129,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -829,11 +878,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="382026016"/>
-        <c:axId val="380003784"/>
+        <c:axId val="335791088"/>
+        <c:axId val="335787952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="382026016"/>
+        <c:axId val="335791088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -879,6 +928,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -945,12 +995,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380003784"/>
+        <c:crossAx val="335787952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="380003784"/>
+        <c:axId val="335787952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,6 +1046,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1062,7 +1113,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382026016"/>
+        <c:crossAx val="335791088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1196,7 +1247,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3774,11 +3824,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="380008096"/>
-        <c:axId val="380005744"/>
+        <c:axId val="335791872"/>
+        <c:axId val="335793440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="380008096"/>
+        <c:axId val="335791872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3824,7 +3874,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3891,12 +3940,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380005744"/>
+        <c:crossAx val="335793440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="380005744"/>
+        <c:axId val="335793440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3942,7 +3991,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4009,7 +4057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380008096"/>
+        <c:crossAx val="335791872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4140,7 +4188,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6718,11 +6765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="380006528"/>
-        <c:axId val="380008488"/>
+        <c:axId val="335793832"/>
+        <c:axId val="335792264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="380006528"/>
+        <c:axId val="335793832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6768,7 +6815,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6835,12 +6881,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380008488"/>
+        <c:crossAx val="335792264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="380008488"/>
+        <c:axId val="335792264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6886,7 +6932,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6953,7 +6998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380006528"/>
+        <c:crossAx val="335793832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7084,7 +7129,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12186,18 +12230,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="380002216"/>
-        <c:axId val="380009272"/>
+        <c:axId val="335793048"/>
+        <c:axId val="335794616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="380002216"/>
+        <c:axId val="335793048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12264,12 +12307,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380009272"/>
+        <c:crossAx val="335794616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="380009272"/>
+        <c:axId val="335794616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12315,7 +12358,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12382,7 +12424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380002216"/>
+        <c:crossAx val="335793048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12513,7 +12555,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15215,11 +15256,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438143384"/>
-        <c:axId val="438144560"/>
+        <c:axId val="440933616"/>
+        <c:axId val="440934792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438143384"/>
+        <c:axId val="440933616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15251,7 +15292,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15318,12 +15358,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438144560"/>
+        <c:crossAx val="440934792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438144560"/>
+        <c:axId val="440934792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -15375,7 +15415,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15442,7 +15481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438143384"/>
+        <c:crossAx val="440933616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15568,7 +15607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18136,11 +18174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438146128"/>
-        <c:axId val="438142992"/>
+        <c:axId val="440935184"/>
+        <c:axId val="440934400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438146128"/>
+        <c:axId val="440935184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18172,7 +18210,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18239,12 +18276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438142992"/>
+        <c:crossAx val="440934400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438142992"/>
+        <c:axId val="440934400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18295,7 +18332,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18362,7 +18398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438146128"/>
+        <c:crossAx val="440935184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18376,7 +18412,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21779,7 +21814,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21845,7 +21880,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8674835" cy="6297521"/>
+    <xdr:ext cx="9294091" cy="6068580"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -23222,8 +23257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O82" sqref="O82"/>
+    <sheetView topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J205" sqref="J205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25886,7 +25921,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>2039</v>
       </c>
@@ -25959,7 +25994,7 @@
       <c r="I45">
         <v>19</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26016,7 +26051,7 @@
       <c r="I46">
         <v>20</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26073,7 +26108,7 @@
       <c r="I47">
         <v>21</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26130,7 +26165,7 @@
       <c r="I48">
         <v>17</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26187,7 +26222,7 @@
       <c r="I49">
         <v>18</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26244,7 +26279,7 @@
       <c r="I50">
         <v>19</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26301,7 +26336,7 @@
       <c r="I51">
         <v>20</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26358,7 +26393,7 @@
       <c r="I52">
         <v>21</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26415,7 +26450,7 @@
       <c r="I53">
         <v>22</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26472,7 +26507,7 @@
       <c r="I54">
         <v>18</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26529,7 +26564,7 @@
       <c r="I55">
         <v>17</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26586,7 +26621,7 @@
       <c r="I56">
         <v>18</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26643,7 +26678,7 @@
       <c r="I57">
         <v>19</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26700,7 +26735,7 @@
       <c r="I58">
         <v>20</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26757,7 +26792,7 @@
       <c r="I59">
         <v>21</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26814,7 +26849,7 @@
       <c r="I60">
         <v>22</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26871,7 +26906,7 @@
       <c r="I61">
         <v>18</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26928,7 +26963,7 @@
       <c r="I62">
         <v>19</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -26985,7 +27020,7 @@
       <c r="I63">
         <v>20</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27042,7 +27077,7 @@
       <c r="I64">
         <v>21</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27099,7 +27134,7 @@
       <c r="I65">
         <v>22</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27156,7 +27191,7 @@
       <c r="I66">
         <v>16</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27213,7 +27248,7 @@
       <c r="I67">
         <v>17</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27270,7 +27305,7 @@
       <c r="I68">
         <v>18</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27327,7 +27362,7 @@
       <c r="I69">
         <v>19</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -27384,7 +27419,7 @@
       <c r="I70">
         <v>20</v>
       </c>
-      <c r="J70">
+      <c r="J70" s="5">
         <f t="shared" ref="J70:J133" si="4">F70-H70</f>
         <v>0</v>
       </c>
@@ -27441,7 +27476,7 @@
       <c r="I71">
         <v>21</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27498,7 +27533,7 @@
       <c r="I72">
         <v>17</v>
       </c>
-      <c r="J72">
+      <c r="J72" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27555,7 +27590,7 @@
       <c r="I73">
         <v>18</v>
       </c>
-      <c r="J73">
+      <c r="J73" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27612,7 +27647,7 @@
       <c r="I74">
         <v>19</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27669,7 +27704,7 @@
       <c r="I75">
         <v>20</v>
       </c>
-      <c r="J75">
+      <c r="J75" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27726,7 +27761,7 @@
       <c r="I76">
         <v>21</v>
       </c>
-      <c r="J76">
+      <c r="J76" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27783,7 +27818,7 @@
       <c r="I77">
         <v>22</v>
       </c>
-      <c r="J77">
+      <c r="J77" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27840,7 +27875,7 @@
       <c r="I78">
         <v>18</v>
       </c>
-      <c r="J78">
+      <c r="J78" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27897,7 +27932,7 @@
       <c r="I79">
         <v>17</v>
       </c>
-      <c r="J79">
+      <c r="J79" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -27954,7 +27989,7 @@
       <c r="I80">
         <v>18</v>
       </c>
-      <c r="J80">
+      <c r="J80" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -28011,7 +28046,7 @@
       <c r="I81">
         <v>19</v>
       </c>
-      <c r="J81">
+      <c r="J81" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28068,7 +28103,7 @@
       <c r="I82">
         <v>20</v>
       </c>
-      <c r="J82">
+      <c r="J82" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28125,7 +28160,7 @@
       <c r="I83">
         <v>21</v>
       </c>
-      <c r="J83">
+      <c r="J83" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28182,7 +28217,7 @@
       <c r="I84">
         <v>22</v>
       </c>
-      <c r="J84">
+      <c r="J84" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28239,7 +28274,7 @@
       <c r="I85">
         <v>18</v>
       </c>
-      <c r="J85">
+      <c r="J85" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28296,7 +28331,7 @@
       <c r="I86">
         <v>19</v>
       </c>
-      <c r="J86">
+      <c r="J86" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28353,7 +28388,7 @@
       <c r="I87">
         <v>20</v>
       </c>
-      <c r="J87">
+      <c r="J87" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28410,7 +28445,7 @@
       <c r="I88">
         <v>21</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28467,7 +28502,7 @@
       <c r="I89">
         <v>22</v>
       </c>
-      <c r="J89">
+      <c r="J89" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28524,7 +28559,7 @@
       <c r="I90">
         <v>23</v>
       </c>
-      <c r="J90">
+      <c r="J90" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28581,7 +28616,7 @@
       <c r="I91">
         <v>19</v>
       </c>
-      <c r="J91">
+      <c r="J91" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28638,7 +28673,7 @@
       <c r="I92">
         <v>18</v>
       </c>
-      <c r="J92">
+      <c r="J92" s="5">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
@@ -28695,7 +28730,7 @@
       <c r="I93">
         <v>19</v>
       </c>
-      <c r="J93">
+      <c r="J93" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -28752,7 +28787,7 @@
       <c r="I94">
         <v>20</v>
       </c>
-      <c r="J94">
+      <c r="J94" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -28809,7 +28844,7 @@
       <c r="I95">
         <v>21</v>
       </c>
-      <c r="J95">
+      <c r="J95" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -28866,7 +28901,7 @@
       <c r="I96">
         <v>22</v>
       </c>
-      <c r="J96">
+      <c r="J96" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -28923,7 +28958,7 @@
       <c r="I97">
         <v>23</v>
       </c>
-      <c r="J97">
+      <c r="J97" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -28980,7 +29015,7 @@
       <c r="I98">
         <v>19</v>
       </c>
-      <c r="J98">
+      <c r="J98" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29037,7 +29072,7 @@
       <c r="I99">
         <v>20</v>
       </c>
-      <c r="J99">
+      <c r="J99" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29094,7 +29129,7 @@
       <c r="I100">
         <v>21</v>
       </c>
-      <c r="J100">
+      <c r="J100" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29151,7 +29186,7 @@
       <c r="I101">
         <v>22</v>
       </c>
-      <c r="J101">
+      <c r="J101" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29208,7 +29243,7 @@
       <c r="I102">
         <v>23</v>
       </c>
-      <c r="J102">
+      <c r="J102" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29265,7 +29300,7 @@
       <c r="I103">
         <v>17</v>
       </c>
-      <c r="J103">
+      <c r="J103" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29306,7 +29341,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E104">
         <v>2099</v>
       </c>
@@ -29322,7 +29357,7 @@
       <c r="I104">
         <v>18</v>
       </c>
-      <c r="J104">
+      <c r="J104" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29379,7 +29414,7 @@
       <c r="I105">
         <v>14</v>
       </c>
-      <c r="J105">
+      <c r="J105" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29436,7 +29471,7 @@
       <c r="I106">
         <v>15</v>
       </c>
-      <c r="J106">
+      <c r="J106" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29470,7 +29505,7 @@
       <c r="I107">
         <v>16</v>
       </c>
-      <c r="J107">
+      <c r="J107" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29504,7 +29539,7 @@
       <c r="I108">
         <v>17</v>
       </c>
-      <c r="J108">
+      <c r="J108" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29538,7 +29573,7 @@
       <c r="I109">
         <v>18</v>
       </c>
-      <c r="J109">
+      <c r="J109" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29572,7 +29607,7 @@
       <c r="I110">
         <v>19</v>
       </c>
-      <c r="J110">
+      <c r="J110" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29606,7 +29641,7 @@
       <c r="I111">
         <v>15</v>
       </c>
-      <c r="J111">
+      <c r="J111" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29640,7 +29675,7 @@
       <c r="I112">
         <v>16</v>
       </c>
-      <c r="J112">
+      <c r="J112" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29674,7 +29709,7 @@
       <c r="I113">
         <v>17</v>
       </c>
-      <c r="J113">
+      <c r="J113" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29708,7 +29743,7 @@
       <c r="I114">
         <v>18</v>
       </c>
-      <c r="J114">
+      <c r="J114" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29742,7 +29777,7 @@
       <c r="I115">
         <v>19</v>
       </c>
-      <c r="J115">
+      <c r="J115" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29776,7 +29811,7 @@
       <c r="I116">
         <v>20</v>
       </c>
-      <c r="J116">
+      <c r="J116" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29810,7 +29845,7 @@
       <c r="I117">
         <v>16</v>
       </c>
-      <c r="J117">
+      <c r="J117" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29844,7 +29879,7 @@
       <c r="I118">
         <v>15</v>
       </c>
-      <c r="J118">
+      <c r="J118" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29878,7 +29913,7 @@
       <c r="I119">
         <v>16</v>
       </c>
-      <c r="J119">
+      <c r="J119" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29912,7 +29947,7 @@
       <c r="I120">
         <v>17</v>
       </c>
-      <c r="J120">
+      <c r="J120" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29946,7 +29981,7 @@
       <c r="I121">
         <v>18</v>
       </c>
-      <c r="J121">
+      <c r="J121" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -29980,7 +30015,7 @@
       <c r="I122">
         <v>19</v>
       </c>
-      <c r="J122">
+      <c r="J122" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30014,7 +30049,7 @@
       <c r="I123">
         <v>20</v>
       </c>
-      <c r="J123">
+      <c r="J123" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30048,7 +30083,7 @@
       <c r="I124">
         <v>16</v>
       </c>
-      <c r="J124">
+      <c r="J124" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30082,7 +30117,7 @@
       <c r="I125">
         <v>17</v>
       </c>
-      <c r="J125">
+      <c r="J125" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30116,7 +30151,7 @@
       <c r="I126">
         <v>18</v>
       </c>
-      <c r="J126">
+      <c r="J126" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30150,7 +30185,7 @@
       <c r="I127">
         <v>19</v>
       </c>
-      <c r="J127">
+      <c r="J127" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30184,7 +30219,7 @@
       <c r="I128">
         <v>20</v>
       </c>
-      <c r="J128">
+      <c r="J128" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30218,7 +30253,7 @@
       <c r="I129">
         <v>21</v>
       </c>
-      <c r="J129">
+      <c r="J129" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30252,7 +30287,7 @@
       <c r="I130">
         <v>17</v>
       </c>
-      <c r="J130">
+      <c r="J130" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30286,7 +30321,7 @@
       <c r="I131">
         <v>16</v>
       </c>
-      <c r="J131">
+      <c r="J131" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30320,7 +30355,7 @@
       <c r="I132">
         <v>17</v>
       </c>
-      <c r="J132">
+      <c r="J132" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30354,7 +30389,7 @@
       <c r="I133">
         <v>18</v>
       </c>
-      <c r="J133">
+      <c r="J133" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -30388,7 +30423,7 @@
       <c r="I134">
         <v>19</v>
       </c>
-      <c r="J134">
+      <c r="J134" s="5">
         <f t="shared" ref="J134:J197" si="8">F134-H134</f>
         <v>0</v>
       </c>
@@ -30422,7 +30457,7 @@
       <c r="I135">
         <v>20</v>
       </c>
-      <c r="J135">
+      <c r="J135" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -30456,7 +30491,7 @@
       <c r="I136">
         <v>21</v>
       </c>
-      <c r="J136">
+      <c r="J136" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -30490,7 +30525,7 @@
       <c r="I137">
         <v>17</v>
       </c>
-      <c r="J137">
+      <c r="J137" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -30524,7 +30559,7 @@
       <c r="I138">
         <v>18</v>
       </c>
-      <c r="J138">
+      <c r="J138" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -30558,7 +30593,7 @@
       <c r="I139">
         <v>19</v>
       </c>
-      <c r="J139">
+      <c r="J139" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -30592,7 +30627,7 @@
       <c r="I140">
         <v>20</v>
       </c>
-      <c r="J140">
+      <c r="J140" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -30626,7 +30661,7 @@
       <c r="I141">
         <v>21</v>
       </c>
-      <c r="J141">
+      <c r="J141" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30660,7 +30695,7 @@
       <c r="I142">
         <v>15</v>
       </c>
-      <c r="J142">
+      <c r="J142" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30694,7 +30729,7 @@
       <c r="I143">
         <v>16</v>
       </c>
-      <c r="J143">
+      <c r="J143" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30728,7 +30763,7 @@
       <c r="I144">
         <v>17</v>
       </c>
-      <c r="J144">
+      <c r="J144" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30762,7 +30797,7 @@
       <c r="I145">
         <v>18</v>
       </c>
-      <c r="J145">
+      <c r="J145" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30796,7 +30831,7 @@
       <c r="I146">
         <v>19</v>
       </c>
-      <c r="J146">
+      <c r="J146" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30830,7 +30865,7 @@
       <c r="I147">
         <v>20</v>
       </c>
-      <c r="J147">
+      <c r="J147" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30864,7 +30899,7 @@
       <c r="I148">
         <v>16</v>
       </c>
-      <c r="J148">
+      <c r="J148" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30898,7 +30933,7 @@
       <c r="I149">
         <v>17</v>
       </c>
-      <c r="J149">
+      <c r="J149" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30932,7 +30967,7 @@
       <c r="I150">
         <v>18</v>
       </c>
-      <c r="J150">
+      <c r="J150" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -30966,7 +31001,7 @@
       <c r="I151">
         <v>19</v>
       </c>
-      <c r="J151">
+      <c r="J151" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -31000,7 +31035,7 @@
       <c r="I152">
         <v>20</v>
       </c>
-      <c r="J152">
+      <c r="J152" s="5">
         <f t="shared" si="8"/>
         <v>-1</v>
       </c>
@@ -31034,7 +31069,7 @@
       <c r="I153">
         <v>21</v>
       </c>
-      <c r="J153">
+      <c r="J153" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31068,7 +31103,7 @@
       <c r="I154">
         <v>17</v>
       </c>
-      <c r="J154">
+      <c r="J154" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31102,7 +31137,7 @@
       <c r="I155">
         <v>16</v>
       </c>
-      <c r="J155">
+      <c r="J155" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31136,7 +31171,7 @@
       <c r="I156">
         <v>17</v>
       </c>
-      <c r="J156">
+      <c r="J156" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31170,7 +31205,7 @@
       <c r="I157">
         <v>18</v>
       </c>
-      <c r="J157">
+      <c r="J157" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31204,7 +31239,7 @@
       <c r="I158">
         <v>19</v>
       </c>
-      <c r="J158">
+      <c r="J158" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31238,7 +31273,7 @@
       <c r="I159">
         <v>20</v>
       </c>
-      <c r="J159">
+      <c r="J159" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31272,7 +31307,7 @@
       <c r="I160">
         <v>21</v>
       </c>
-      <c r="J160">
+      <c r="J160" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31306,7 +31341,7 @@
       <c r="I161">
         <v>17</v>
       </c>
-      <c r="J161">
+      <c r="J161" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31340,7 +31375,7 @@
       <c r="I162">
         <v>18</v>
       </c>
-      <c r="J162">
+      <c r="J162" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31374,7 +31409,7 @@
       <c r="I163">
         <v>19</v>
       </c>
-      <c r="J163">
+      <c r="J163" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -31392,7 +31427,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="164" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E164">
         <v>2159</v>
       </c>
@@ -31408,7 +31443,7 @@
       <c r="I164">
         <v>20</v>
       </c>
-      <c r="J164">
+      <c r="J164" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -32822,20 +32857,1689 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J5:J205">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:L205">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:S105">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1980</v>
+      </c>
+      <c r="D3">
+        <v>2040</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2100</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2160</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1981</v>
+      </c>
+      <c r="D4">
+        <v>2041</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2101</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2161</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1982</v>
+      </c>
+      <c r="D5">
+        <v>2042</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2102</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>2162</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1983</v>
+      </c>
+      <c r="D6">
+        <v>2043</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2103</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>2163</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1984</v>
+      </c>
+      <c r="D7">
+        <v>2044</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2104</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2164</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1985</v>
+      </c>
+      <c r="D8">
+        <v>2045</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2105</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>2165</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1986</v>
+      </c>
+      <c r="D9">
+        <v>2046</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2106</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>2166</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1987</v>
+      </c>
+      <c r="D10">
+        <v>2047</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2107</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>2167</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1988</v>
+      </c>
+      <c r="D11">
+        <v>2048</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>2108</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2168</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1989</v>
+      </c>
+      <c r="D12">
+        <v>2049</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2109</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2169</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1990</v>
+      </c>
+      <c r="D13">
+        <v>2050</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>2110</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>2170</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1991</v>
+      </c>
+      <c r="D14">
+        <v>2051</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>2111</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>2171</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>1992</v>
+      </c>
+      <c r="D15">
+        <v>2052</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2112</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>2172</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>1993</v>
+      </c>
+      <c r="D16">
+        <v>2053</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2113</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>2173</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>1994</v>
+      </c>
+      <c r="D17">
+        <v>2054</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2114</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>2174</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>1995</v>
+      </c>
+      <c r="D18">
+        <v>2055</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>2115</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2175</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>1996</v>
+      </c>
+      <c r="D19">
+        <v>2056</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2116</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2176</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>1997</v>
+      </c>
+      <c r="D20">
+        <v>2057</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2117</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>2177</v>
+      </c>
+      <c r="I20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>1998</v>
+      </c>
+      <c r="D21">
+        <v>2058</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>2118</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2178</v>
+      </c>
+      <c r="I21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1999</v>
+      </c>
+      <c r="D22">
+        <v>2059</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>2119</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2179</v>
+      </c>
+      <c r="I22" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>2060</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2120</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2180</v>
+      </c>
+      <c r="I23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>2001</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>2061</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2121</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>2181</v>
+      </c>
+      <c r="I24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>2002</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>2062</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2122</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>2182</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>2003</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>2063</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>2123</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>2183</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>2004</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>2064</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>2124</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>2184</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>2005</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>2065</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>2125</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>2185</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>2006</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>2066</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>2126</v>
+      </c>
+      <c r="G29" s="7">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>2186</v>
+      </c>
+      <c r="I29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>2007</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>2067</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>2127</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>2187</v>
+      </c>
+      <c r="I30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>2008</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>2068</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>2128</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>2188</v>
+      </c>
+      <c r="I31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>2009</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>2069</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>2129</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>2189</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>2010</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>2070</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>2130</v>
+      </c>
+      <c r="G33" s="7">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>2190</v>
+      </c>
+      <c r="I33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>2011</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>2071</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>2131</v>
+      </c>
+      <c r="G34" s="7">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>2191</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>2012</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>2072</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>2132</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>2192</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>2013</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>2073</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>2133</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>2193</v>
+      </c>
+      <c r="I36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>2014</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>2074</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>2134</v>
+      </c>
+      <c r="G37" s="7">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>2194</v>
+      </c>
+      <c r="I37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>2015</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>2075</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>2135</v>
+      </c>
+      <c r="G38" s="7">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>2195</v>
+      </c>
+      <c r="I38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>2016</v>
+      </c>
+      <c r="C39" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>2076</v>
+      </c>
+      <c r="E39" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F39">
+        <v>2136</v>
+      </c>
+      <c r="G39" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H39">
+        <v>2196</v>
+      </c>
+      <c r="I39" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>2017</v>
+      </c>
+      <c r="C40" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D40">
+        <v>2077</v>
+      </c>
+      <c r="E40" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F40">
+        <v>2137</v>
+      </c>
+      <c r="G40" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H40">
+        <v>2197</v>
+      </c>
+      <c r="I40" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>2018</v>
+      </c>
+      <c r="C41" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D41">
+        <v>2078</v>
+      </c>
+      <c r="E41" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F41">
+        <v>2138</v>
+      </c>
+      <c r="G41" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H41">
+        <v>2198</v>
+      </c>
+      <c r="I41" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>2019</v>
+      </c>
+      <c r="C42" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D42">
+        <v>2079</v>
+      </c>
+      <c r="E42" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F42">
+        <v>2139</v>
+      </c>
+      <c r="G42" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H42">
+        <v>2199</v>
+      </c>
+      <c r="I42" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>2020</v>
+      </c>
+      <c r="C43" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D43">
+        <v>2080</v>
+      </c>
+      <c r="E43" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F43">
+        <v>2140</v>
+      </c>
+      <c r="G43" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H43" s="7">
+        <v>2200</v>
+      </c>
+      <c r="I43" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>2021</v>
+      </c>
+      <c r="C44" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D44">
+        <v>2081</v>
+      </c>
+      <c r="E44" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F44">
+        <v>2141</v>
+      </c>
+      <c r="G44" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H44">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>2022</v>
+      </c>
+      <c r="C45" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D45">
+        <v>2082</v>
+      </c>
+      <c r="E45" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F45">
+        <v>2142</v>
+      </c>
+      <c r="G45" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H45">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>2023</v>
+      </c>
+      <c r="C46" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D46">
+        <v>2083</v>
+      </c>
+      <c r="E46" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F46">
+        <v>2143</v>
+      </c>
+      <c r="G46" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H46">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>2024</v>
+      </c>
+      <c r="C47" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D47">
+        <v>2084</v>
+      </c>
+      <c r="E47" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F47">
+        <v>2144</v>
+      </c>
+      <c r="G47" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H47">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>2025</v>
+      </c>
+      <c r="C48" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D48">
+        <v>2085</v>
+      </c>
+      <c r="E48" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F48">
+        <v>2145</v>
+      </c>
+      <c r="G48" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H48">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>2026</v>
+      </c>
+      <c r="C49" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D49">
+        <v>2086</v>
+      </c>
+      <c r="E49" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F49">
+        <v>2146</v>
+      </c>
+      <c r="G49" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H49">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>2027</v>
+      </c>
+      <c r="C50" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D50">
+        <v>2087</v>
+      </c>
+      <c r="E50" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F50">
+        <v>2147</v>
+      </c>
+      <c r="G50" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H50">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>2028</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>2088</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>2148</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <v>2029</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>2089</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>2149</v>
+      </c>
+      <c r="G52" s="7">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>2030</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>2090</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>2150</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <v>2031</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>2091</v>
+      </c>
+      <c r="E54" s="7">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>2151</v>
+      </c>
+      <c r="G54" s="7">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>2032</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>2092</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>2152</v>
+      </c>
+      <c r="G55" s="7">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>2033</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2093</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>2153</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>2034</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2094</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>2154</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>2095</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>2155</v>
+      </c>
+      <c r="G58" s="7">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>2036</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2096</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>2156</v>
+      </c>
+      <c r="G59" s="7">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>2037</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>2097</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>2157</v>
+      </c>
+      <c r="G60" s="7">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>2038</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>2098</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>2158</v>
+      </c>
+      <c r="G61" s="7">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>2039</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>2099</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>2159</v>
+      </c>
+      <c r="G62" s="7">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>2219</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor tweak to the main.py so it will, created new expStats for sets with smaller A for slow
</commit_message>
<xml_diff>
--- a/consolidated_data.xlsx
+++ b/consolidated_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="103" windowWidth="14803" windowHeight="8014" tabRatio="722" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="2" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Q6" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
     <sheet name="Comparing differences A mod 60" sheetId="18" r:id="rId8"/>
+    <sheet name="Comparing differences Q5 V2" sheetId="19" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>DP</t>
   </si>
@@ -186,37 +187,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -878,11 +849,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335791088"/>
-        <c:axId val="335787952"/>
+        <c:axId val="325631880"/>
+        <c:axId val="325627176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335791088"/>
+        <c:axId val="325631880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,7 +899,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -995,12 +965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335787952"/>
+        <c:crossAx val="325627176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335787952"/>
+        <c:axId val="325627176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1016,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1113,7 +1082,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335791088"/>
+        <c:crossAx val="325631880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3824,11 +3793,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335791872"/>
-        <c:axId val="335793440"/>
+        <c:axId val="325630312"/>
+        <c:axId val="325629136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335791872"/>
+        <c:axId val="325630312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3940,12 +3909,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335793440"/>
+        <c:crossAx val="325629136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335793440"/>
+        <c:axId val="325629136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4057,7 +4026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335791872"/>
+        <c:crossAx val="325630312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6765,11 +6734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335793832"/>
-        <c:axId val="335792264"/>
+        <c:axId val="325626000"/>
+        <c:axId val="325629528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335793832"/>
+        <c:axId val="325626000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6881,12 +6850,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335792264"/>
+        <c:crossAx val="325629528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335792264"/>
+        <c:axId val="325629528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6998,7 +6967,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335793832"/>
+        <c:crossAx val="325626000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12230,11 +12199,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335793048"/>
-        <c:axId val="335794616"/>
+        <c:axId val="325628352"/>
+        <c:axId val="435293168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335793048"/>
+        <c:axId val="325628352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12307,12 +12276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335794616"/>
+        <c:crossAx val="435293168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335794616"/>
+        <c:axId val="435293168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12424,7 +12393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335793048"/>
+        <c:crossAx val="325628352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15256,11 +15225,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="440933616"/>
-        <c:axId val="440934792"/>
+        <c:axId val="435291992"/>
+        <c:axId val="435294344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="440933616"/>
+        <c:axId val="435291992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15358,12 +15327,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440934792"/>
+        <c:crossAx val="435294344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="440934792"/>
+        <c:axId val="435294344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -15481,7 +15450,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440933616"/>
+        <c:crossAx val="435291992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18174,11 +18143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="440935184"/>
-        <c:axId val="440934400"/>
+        <c:axId val="435296304"/>
+        <c:axId val="435290424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="440935184"/>
+        <c:axId val="435296304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18276,12 +18245,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440934400"/>
+        <c:crossAx val="435290424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="440934400"/>
+        <c:axId val="435290424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18398,7 +18367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440935184"/>
+        <c:crossAx val="435296304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23257,24 +23226,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W205"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J205" sqref="J205"/>
+    <sheetView topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:K205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.53515625" customWidth="1"/>
+    <col min="7" max="7" width="8.3828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.69140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.3828125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -23303,7 +23272,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -23347,7 +23316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -23413,7 +23382,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -23479,7 +23448,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -23545,7 +23514,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -23611,7 +23580,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -23677,7 +23646,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>2035</v>
       </c>
@@ -23743,7 +23712,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2040</v>
       </c>
@@ -23809,7 +23778,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>2045</v>
       </c>
@@ -23875,7 +23844,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2050</v>
       </c>
@@ -23941,7 +23910,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>2055</v>
       </c>
@@ -24007,7 +23976,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2060</v>
       </c>
@@ -24073,7 +24042,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2065</v>
       </c>
@@ -24139,7 +24108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2070</v>
       </c>
@@ -24205,7 +24174,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>2075</v>
       </c>
@@ -24271,7 +24240,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2080</v>
       </c>
@@ -24337,7 +24306,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>2085</v>
       </c>
@@ -24403,7 +24372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2090</v>
       </c>
@@ -24469,7 +24438,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>2095</v>
       </c>
@@ -24535,7 +24504,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2100</v>
       </c>
@@ -24601,7 +24570,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>2105</v>
       </c>
@@ -24667,7 +24636,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2110</v>
       </c>
@@ -24733,7 +24702,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>2115</v>
       </c>
@@ -24799,7 +24768,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2120</v>
       </c>
@@ -24865,7 +24834,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>2125</v>
       </c>
@@ -24931,7 +24900,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>2130</v>
       </c>
@@ -24997,7 +24966,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>2135</v>
       </c>
@@ -25063,7 +25032,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2140</v>
       </c>
@@ -25129,7 +25098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>2145</v>
       </c>
@@ -25195,7 +25164,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>2150</v>
       </c>
@@ -25261,7 +25230,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>2155</v>
       </c>
@@ -25327,7 +25296,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>2160</v>
       </c>
@@ -25393,7 +25362,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>2165</v>
       </c>
@@ -25459,7 +25428,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>2170</v>
       </c>
@@ -25525,7 +25494,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>2175</v>
       </c>
@@ -25591,7 +25560,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>2180</v>
       </c>
@@ -25657,7 +25626,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>2185</v>
       </c>
@@ -25723,7 +25692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>2190</v>
       </c>
@@ -25789,7 +25758,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>2195</v>
       </c>
@@ -25855,7 +25824,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>2200</v>
       </c>
@@ -25921,7 +25890,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E44">
         <v>2039</v>
       </c>
@@ -25978,7 +25947,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.4">
       <c r="E45">
         <v>2040</v>
       </c>
@@ -26035,7 +26004,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.4">
       <c r="E46">
         <v>2041</v>
       </c>
@@ -26092,7 +26061,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.4">
       <c r="E47">
         <v>2042</v>
       </c>
@@ -26149,7 +26118,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.4">
       <c r="E48">
         <v>2043</v>
       </c>
@@ -26206,7 +26175,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E49">
         <v>2044</v>
       </c>
@@ -26263,7 +26232,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E50">
         <v>2045</v>
       </c>
@@ -26320,7 +26289,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E51">
         <v>2046</v>
       </c>
@@ -26377,7 +26346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E52">
         <v>2047</v>
       </c>
@@ -26434,7 +26403,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E53">
         <v>2048</v>
       </c>
@@ -26491,7 +26460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E54">
         <v>2049</v>
       </c>
@@ -26548,7 +26517,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E55">
         <v>2050</v>
       </c>
@@ -26605,7 +26574,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E56">
         <v>2051</v>
       </c>
@@ -26662,7 +26631,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E57">
         <v>2052</v>
       </c>
@@ -26719,7 +26688,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E58">
         <v>2053</v>
       </c>
@@ -26776,7 +26745,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E59">
         <v>2054</v>
       </c>
@@ -26833,7 +26802,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E60">
         <v>2055</v>
       </c>
@@ -26890,7 +26859,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E61">
         <v>2056</v>
       </c>
@@ -26947,7 +26916,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E62">
         <v>2057</v>
       </c>
@@ -27004,7 +26973,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E63">
         <v>2058</v>
       </c>
@@ -27061,7 +27030,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E64">
         <v>2059</v>
       </c>
@@ -27118,7 +27087,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E65">
         <v>2060</v>
       </c>
@@ -27175,7 +27144,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E66">
         <v>2061</v>
       </c>
@@ -27232,7 +27201,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E67">
         <v>2062</v>
       </c>
@@ -27289,7 +27258,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E68">
         <v>2063</v>
       </c>
@@ -27346,7 +27315,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E69">
         <v>2064</v>
       </c>
@@ -27403,7 +27372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E70">
         <v>2065</v>
       </c>
@@ -27460,7 +27429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E71">
         <v>2066</v>
       </c>
@@ -27517,7 +27486,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E72">
         <v>2067</v>
       </c>
@@ -27574,7 +27543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E73">
         <v>2068</v>
       </c>
@@ -27631,7 +27600,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E74">
         <v>2069</v>
       </c>
@@ -27688,7 +27657,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E75">
         <v>2070</v>
       </c>
@@ -27745,7 +27714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E76">
         <v>2071</v>
       </c>
@@ -27802,7 +27771,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E77">
         <v>2072</v>
       </c>
@@ -27859,7 +27828,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E78">
         <v>2073</v>
       </c>
@@ -27916,7 +27885,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E79">
         <v>2074</v>
       </c>
@@ -27973,7 +27942,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E80">
         <v>2075</v>
       </c>
@@ -28030,7 +27999,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E81">
         <v>2076</v>
       </c>
@@ -28087,7 +28056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E82">
         <v>2077</v>
       </c>
@@ -28144,7 +28113,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E83">
         <v>2078</v>
       </c>
@@ -28201,7 +28170,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E84">
         <v>2079</v>
       </c>
@@ -28258,7 +28227,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E85">
         <v>2080</v>
       </c>
@@ -28315,7 +28284,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E86">
         <v>2081</v>
       </c>
@@ -28372,7 +28341,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E87">
         <v>2082</v>
       </c>
@@ -28429,7 +28398,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E88">
         <v>2083</v>
       </c>
@@ -28486,7 +28455,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E89">
         <v>2084</v>
       </c>
@@ -28543,7 +28512,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E90">
         <v>2085</v>
       </c>
@@ -28600,7 +28569,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E91">
         <v>2086</v>
       </c>
@@ -28657,7 +28626,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E92">
         <v>2087</v>
       </c>
@@ -28714,7 +28683,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E93">
         <v>2088</v>
       </c>
@@ -28771,7 +28740,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E94">
         <v>2089</v>
       </c>
@@ -28828,7 +28797,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E95">
         <v>2090</v>
       </c>
@@ -28885,7 +28854,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E96">
         <v>2091</v>
       </c>
@@ -28942,7 +28911,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E97">
         <v>2092</v>
       </c>
@@ -28999,7 +28968,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E98">
         <v>2093</v>
       </c>
@@ -29056,7 +29025,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E99">
         <v>2094</v>
       </c>
@@ -29113,7 +29082,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E100">
         <v>2095</v>
       </c>
@@ -29170,7 +29139,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E101">
         <v>2096</v>
       </c>
@@ -29227,7 +29196,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E102">
         <v>2097</v>
       </c>
@@ -29284,7 +29253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E103">
         <v>2098</v>
       </c>
@@ -29341,7 +29310,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E104">
         <v>2099</v>
       </c>
@@ -29398,7 +29367,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E105">
         <v>2100</v>
       </c>
@@ -29455,7 +29424,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E106">
         <v>2101</v>
       </c>
@@ -29489,7 +29458,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E107">
         <v>2102</v>
       </c>
@@ -29523,7 +29492,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E108">
         <v>2103</v>
       </c>
@@ -29557,7 +29526,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E109">
         <v>2104</v>
       </c>
@@ -29591,7 +29560,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E110">
         <v>2105</v>
       </c>
@@ -29625,7 +29594,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E111">
         <v>2106</v>
       </c>
@@ -29659,7 +29628,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E112">
         <v>2107</v>
       </c>
@@ -29693,7 +29662,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E113">
         <v>2108</v>
       </c>
@@ -29727,7 +29696,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E114">
         <v>2109</v>
       </c>
@@ -29761,7 +29730,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E115">
         <v>2110</v>
       </c>
@@ -29795,7 +29764,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E116">
         <v>2111</v>
       </c>
@@ -29829,7 +29798,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E117">
         <v>2112</v>
       </c>
@@ -29863,7 +29832,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E118">
         <v>2113</v>
       </c>
@@ -29897,7 +29866,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E119">
         <v>2114</v>
       </c>
@@ -29931,7 +29900,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="120" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E120">
         <v>2115</v>
       </c>
@@ -29965,7 +29934,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E121">
         <v>2116</v>
       </c>
@@ -29999,7 +29968,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E122">
         <v>2117</v>
       </c>
@@ -30033,7 +30002,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E123">
         <v>2118</v>
       </c>
@@ -30067,7 +30036,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="124" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E124">
         <v>2119</v>
       </c>
@@ -30101,7 +30070,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="125" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E125">
         <v>2120</v>
       </c>
@@ -30135,7 +30104,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="126" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E126">
         <v>2121</v>
       </c>
@@ -30169,7 +30138,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E127">
         <v>2122</v>
       </c>
@@ -30203,7 +30172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="128" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E128">
         <v>2123</v>
       </c>
@@ -30237,7 +30206,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E129">
         <v>2124</v>
       </c>
@@ -30271,7 +30240,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="130" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E130">
         <v>2125</v>
       </c>
@@ -30305,7 +30274,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E131">
         <v>2126</v>
       </c>
@@ -30339,7 +30308,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="132" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E132">
         <v>2127</v>
       </c>
@@ -30373,7 +30342,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="133" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E133">
         <v>2128</v>
       </c>
@@ -30407,7 +30376,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="134" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E134">
         <v>2129</v>
       </c>
@@ -30441,7 +30410,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="135" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E135">
         <v>2130</v>
       </c>
@@ -30475,7 +30444,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="136" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E136">
         <v>2131</v>
       </c>
@@ -30509,7 +30478,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="137" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E137">
         <v>2132</v>
       </c>
@@ -30543,7 +30512,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="138" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E138">
         <v>2133</v>
       </c>
@@ -30577,7 +30546,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="139" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E139">
         <v>2134</v>
       </c>
@@ -30611,7 +30580,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="140" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E140">
         <v>2135</v>
       </c>
@@ -30645,7 +30614,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="141" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E141">
         <v>2136</v>
       </c>
@@ -30679,7 +30648,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="142" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E142">
         <v>2137</v>
       </c>
@@ -30713,7 +30682,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="143" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E143">
         <v>2138</v>
       </c>
@@ -30747,7 +30716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="144" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E144">
         <v>2139</v>
       </c>
@@ -30781,7 +30750,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="145" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E145">
         <v>2140</v>
       </c>
@@ -30815,7 +30784,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="146" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E146">
         <v>2141</v>
       </c>
@@ -30849,7 +30818,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="147" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E147">
         <v>2142</v>
       </c>
@@ -30883,7 +30852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="148" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E148">
         <v>2143</v>
       </c>
@@ -30917,7 +30886,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="149" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E149">
         <v>2144</v>
       </c>
@@ -30951,7 +30920,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="150" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E150">
         <v>2145</v>
       </c>
@@ -30985,7 +30954,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="151" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E151">
         <v>2146</v>
       </c>
@@ -31019,7 +30988,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="152" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E152">
         <v>2147</v>
       </c>
@@ -31053,7 +31022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="153" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E153">
         <v>2148</v>
       </c>
@@ -31087,7 +31056,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="154" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E154">
         <v>2149</v>
       </c>
@@ -31121,7 +31090,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="155" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E155">
         <v>2150</v>
       </c>
@@ -31155,7 +31124,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="156" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E156">
         <v>2151</v>
       </c>
@@ -31189,7 +31158,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="157" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E157">
         <v>2152</v>
       </c>
@@ -31223,7 +31192,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="158" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E158">
         <v>2153</v>
       </c>
@@ -31257,7 +31226,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="159" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E159">
         <v>2154</v>
       </c>
@@ -31291,7 +31260,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="160" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E160">
         <v>2155</v>
       </c>
@@ -31325,7 +31294,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="161" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E161">
         <v>2156</v>
       </c>
@@ -31359,7 +31328,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="162" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E162">
         <v>2157</v>
       </c>
@@ -31393,7 +31362,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="163" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E163">
         <v>2158</v>
       </c>
@@ -31427,7 +31396,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="164" spans="5:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E164">
         <v>2159</v>
       </c>
@@ -31461,7 +31430,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="165" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E165">
         <v>2160</v>
       </c>
@@ -31495,7 +31464,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="166" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E166">
         <v>2161</v>
       </c>
@@ -31529,7 +31498,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="167" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E167">
         <v>2162</v>
       </c>
@@ -31563,7 +31532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="168" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E168">
         <v>2163</v>
       </c>
@@ -31597,7 +31566,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E169">
         <v>2164</v>
       </c>
@@ -31631,7 +31600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="170" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E170">
         <v>2165</v>
       </c>
@@ -31665,7 +31634,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="171" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E171">
         <v>2166</v>
       </c>
@@ -31699,7 +31668,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="172" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E172">
         <v>2167</v>
       </c>
@@ -31733,7 +31702,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="173" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E173">
         <v>2168</v>
       </c>
@@ -31767,7 +31736,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="174" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E174">
         <v>2169</v>
       </c>
@@ -31801,7 +31770,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E175">
         <v>2170</v>
       </c>
@@ -31835,7 +31804,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="176" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E176">
         <v>2171</v>
       </c>
@@ -31869,7 +31838,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="177" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E177">
         <v>2172</v>
       </c>
@@ -31903,7 +31872,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="178" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E178">
         <v>2173</v>
       </c>
@@ -31937,7 +31906,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="179" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E179">
         <v>2174</v>
       </c>
@@ -31971,7 +31940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="180" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E180">
         <v>2175</v>
       </c>
@@ -32005,7 +31974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="181" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E181">
         <v>2176</v>
       </c>
@@ -32039,7 +32008,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="182" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E182">
         <v>2177</v>
       </c>
@@ -32073,7 +32042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E183">
         <v>2178</v>
       </c>
@@ -32107,7 +32076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="184" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E184">
         <v>2179</v>
       </c>
@@ -32141,7 +32110,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="185" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E185">
         <v>2180</v>
       </c>
@@ -32175,7 +32144,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="186" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E186">
         <v>2181</v>
       </c>
@@ -32209,7 +32178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="187" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E187">
         <v>2182</v>
       </c>
@@ -32243,7 +32212,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="188" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E188">
         <v>2183</v>
       </c>
@@ -32277,7 +32246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="189" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E189">
         <v>2184</v>
       </c>
@@ -32311,7 +32280,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="190" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E190">
         <v>2185</v>
       </c>
@@ -32345,7 +32314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="191" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E191">
         <v>2186</v>
       </c>
@@ -32379,7 +32348,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="192" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E192">
         <v>2187</v>
       </c>
@@ -32413,7 +32382,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="193" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E193">
         <v>2188</v>
       </c>
@@ -32447,7 +32416,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="194" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E194">
         <v>2189</v>
       </c>
@@ -32481,7 +32450,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="195" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E195">
         <v>2190</v>
       </c>
@@ -32515,7 +32484,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="196" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E196">
         <v>2191</v>
       </c>
@@ -32549,7 +32518,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="197" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E197">
         <v>2192</v>
       </c>
@@ -32583,7 +32552,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="198" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E198">
         <v>2193</v>
       </c>
@@ -32617,7 +32586,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="199" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E199">
         <v>2194</v>
       </c>
@@ -32651,7 +32620,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="200" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E200">
         <v>2195</v>
       </c>
@@ -32685,7 +32654,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="201" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E201">
         <v>2196</v>
       </c>
@@ -32719,7 +32688,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="202" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E202">
         <v>2197</v>
       </c>
@@ -32753,7 +32722,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="203" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E203">
         <v>2198</v>
       </c>
@@ -32787,7 +32756,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="204" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E204">
         <v>2199</v>
       </c>
@@ -32821,7 +32790,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="205" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:23" x14ac:dyDescent="0.4">
       <c r="E205">
         <v>2200</v>
       </c>
@@ -32857,17 +32826,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J5:J205">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:L205">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:S105">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32879,24 +32848,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.69140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.69140625" customWidth="1"/>
+    <col min="5" max="5" width="9.69140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.69140625" customWidth="1"/>
+    <col min="7" max="7" width="9.69140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.69140625" customWidth="1"/>
+    <col min="9" max="9" width="9.69140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
@@ -32908,12 +32877,12 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7">
         <v>0</v>
       </c>
@@ -32939,7 +32908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -32965,7 +32934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -32991,7 +32960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -33017,7 +32986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -33043,7 +33012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -33069,7 +33038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -33095,7 +33064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -33121,7 +33090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -33147,7 +33116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -33173,7 +33142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -33199,7 +33168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -33225,7 +33194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -33251,7 +33220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -33277,7 +33246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -33303,7 +33272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -33329,7 +33298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -33355,7 +33324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -33381,7 +33350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -33407,7 +33376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -33433,7 +33402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -33462,7 +33431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -33491,7 +33460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -33520,7 +33489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="7">
         <v>23</v>
       </c>
@@ -33549,7 +33518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -33578,7 +33547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="7">
         <v>25</v>
       </c>
@@ -33607,7 +33576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -33636,7 +33605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="7">
         <v>27</v>
       </c>
@@ -33665,7 +33634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -33694,7 +33663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="7">
         <v>29</v>
       </c>
@@ -33723,7 +33692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -33752,7 +33721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="7">
         <v>31</v>
       </c>
@@ -33781,7 +33750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -33810,7 +33779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="7">
         <v>33</v>
       </c>
@@ -33839,7 +33808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -33868,7 +33837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="7">
         <v>35</v>
       </c>
@@ -33897,7 +33866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="7">
         <v>36</v>
       </c>
@@ -33926,7 +33895,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="7">
         <v>37</v>
       </c>
@@ -33955,7 +33924,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="7">
         <v>38</v>
       </c>
@@ -33984,7 +33953,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="7">
         <v>39</v>
       </c>
@@ -34013,7 +33982,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="7">
         <v>40</v>
       </c>
@@ -34042,7 +34011,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="7">
         <v>41</v>
       </c>
@@ -34068,7 +34037,7 @@
         <v>2201</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="7">
         <v>42</v>
       </c>
@@ -34094,7 +34063,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="7">
         <v>43</v>
       </c>
@@ -34120,7 +34089,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="7">
         <v>44</v>
       </c>
@@ -34146,7 +34115,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="7">
         <v>45</v>
       </c>
@@ -34172,7 +34141,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="7">
         <v>46</v>
       </c>
@@ -34198,7 +34167,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="7">
         <v>47</v>
       </c>
@@ -34224,7 +34193,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="7">
         <v>48</v>
       </c>
@@ -34250,7 +34219,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="7">
         <v>49</v>
       </c>
@@ -34276,7 +34245,7 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="7">
         <v>50</v>
       </c>
@@ -34302,7 +34271,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="7">
         <v>51</v>
       </c>
@@ -34328,7 +34297,7 @@
         <v>2211</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="7">
         <v>52</v>
       </c>
@@ -34354,7 +34323,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="7">
         <v>53</v>
       </c>
@@ -34380,7 +34349,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="7">
         <v>54</v>
       </c>
@@ -34406,7 +34375,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="7">
         <v>55</v>
       </c>
@@ -34432,7 +34401,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="7">
         <v>56</v>
       </c>
@@ -34458,7 +34427,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="7">
         <v>57</v>
       </c>
@@ -34484,7 +34453,7 @@
         <v>2217</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A61" s="7">
         <v>58</v>
       </c>
@@ -34510,7 +34479,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A62" s="7">
         <v>59</v>
       </c>
@@ -34542,4 +34511,1983 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="15.53515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2100</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2101</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2102</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2103</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2104</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2105</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>2106</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>2107</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>2108</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2109</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>2110</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>2111</v>
+      </c>
+      <c r="E13">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>2112</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>2113</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>2114</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>2115</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>2116</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>2117</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>2118</v>
+      </c>
+      <c r="E20">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>2119</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>2120</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>2121</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>2122</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>2123</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>2124</v>
+      </c>
+      <c r="E26">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>2125</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>2126</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>2127</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>2128</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>2129</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>2130</v>
+      </c>
+      <c r="E32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>2131</v>
+      </c>
+      <c r="E33">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>2132</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <v>2133</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <v>2134</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <v>2135</v>
+      </c>
+      <c r="E37">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <v>2136</v>
+      </c>
+      <c r="E38">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="D39">
+        <v>2137</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <v>2138</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <v>2139</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <v>2140</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <v>2141</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <v>2142</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="D45">
+        <v>2143</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="D46">
+        <v>2144</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>2145</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <v>2146</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <v>2147</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="D50">
+        <v>2148</v>
+      </c>
+      <c r="E50">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <v>2149</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>2000</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>2150</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>2001</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>2151</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>2002</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>2152</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>2003</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>2153</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>2004</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2154</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>2005</v>
+      </c>
+      <c r="C57">
+        <v>-3</v>
+      </c>
+      <c r="D57">
+        <v>2155</v>
+      </c>
+      <c r="E57">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>2006</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>2156</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>2007</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2157</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>2008</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>2158</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>2009</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>2159</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>2010</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>2160</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>2011</v>
+      </c>
+      <c r="C63">
+        <v>-3</v>
+      </c>
+      <c r="D63">
+        <v>2161</v>
+      </c>
+      <c r="E63">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>2012</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>2162</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>2013</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>2163</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>2014</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>2164</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>2015</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>2165</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>2016</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>2166</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>2017</v>
+      </c>
+      <c r="C69">
+        <v>-1</v>
+      </c>
+      <c r="D69">
+        <v>2167</v>
+      </c>
+      <c r="E69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>2018</v>
+      </c>
+      <c r="C70">
+        <v>-3</v>
+      </c>
+      <c r="D70">
+        <v>2168</v>
+      </c>
+      <c r="E70">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>2019</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>2169</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>2020</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>2170</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>2021</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>2171</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>2022</v>
+      </c>
+      <c r="C74">
+        <v>-2</v>
+      </c>
+      <c r="D74">
+        <v>2172</v>
+      </c>
+      <c r="E74">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>2023</v>
+      </c>
+      <c r="C75">
+        <v>-2</v>
+      </c>
+      <c r="D75">
+        <v>2173</v>
+      </c>
+      <c r="E75">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>2024</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>2174</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>2025</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>2175</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>2026</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>2176</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>2027</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>2177</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>2028</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>2178</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>2029</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>2179</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>2030</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>2180</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>2031</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>2181</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>2032</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>2182</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>2033</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>2183</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>2034</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>2184</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>2035</v>
+      </c>
+      <c r="C87">
+        <v>-2</v>
+      </c>
+      <c r="D87">
+        <v>2185</v>
+      </c>
+      <c r="E87">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>2036</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>2186</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>2037</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>2187</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>2038</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>2188</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>2039</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>2189</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>2040</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>2190</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>2041</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>2191</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>2042</v>
+      </c>
+      <c r="C94">
+        <v>-3</v>
+      </c>
+      <c r="D94">
+        <v>2192</v>
+      </c>
+      <c r="E94">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>2043</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>2193</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>2044</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>2194</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>2045</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>2195</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>2046</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>2196</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>2047</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>2197</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>2048</v>
+      </c>
+      <c r="C100">
+        <v>-3</v>
+      </c>
+      <c r="D100">
+        <v>2198</v>
+      </c>
+      <c r="E100">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>2049</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>2199</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>2050</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>2200</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>2051</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>2052</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>2053</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>2054</v>
+      </c>
+      <c r="C106">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>2055</v>
+      </c>
+      <c r="C107">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>2056</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>2057</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>2058</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>2059</v>
+      </c>
+      <c r="C111">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>2060</v>
+      </c>
+      <c r="C112">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>2061</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>2062</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>2063</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>2064</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>2065</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>2066</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>2067</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>2068</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>2069</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>2070</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>2071</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>2072</v>
+      </c>
+      <c r="C124">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>2073</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>2074</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>2075</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>2076</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>2077</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>2078</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>2079</v>
+      </c>
+      <c r="C131">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>2080</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>2081</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>2082</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>2083</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>2084</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>2085</v>
+      </c>
+      <c r="C137">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>2086</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>2087</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>2088</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>2089</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>2090</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>2091</v>
+      </c>
+      <c r="C143">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>2092</v>
+      </c>
+      <c r="C144">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>2093</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>2094</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>2095</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>2096</v>
+      </c>
+      <c r="C148">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>2097</v>
+      </c>
+      <c r="C149">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>2098</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>2099</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>